<commit_message>
pridal som triedy na uchovavanie dat z roznych miest, napr. pre technicke udaje...a tiez ich urobil serializovatelne a pridal aj triedu, ktora bude mat ulozene vsetky udaje z appky
</commit_message>
<xml_diff>
--- a/grafikon.xlsx
+++ b/grafikon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>TECHNICAL CHARACTERISTICS OF THE FLOW</t>
   </si>
@@ -20,49 +20,43 @@
     <t>Application date</t>
   </si>
   <si>
-    <t>23.10.2020</t>
+    <t>1234</t>
   </si>
   <si>
     <t>THIS FLOW WILL START BY A</t>
   </si>
   <si>
-    <t>IMPORT</t>
+    <t>asdas</t>
   </si>
   <si>
     <t>Km EXPORT</t>
   </si>
   <si>
-    <t>3103 km</t>
+    <t>10</t>
   </si>
   <si>
     <t>HEIGHT OF THE GOODS</t>
   </si>
   <si>
-    <t>2.73 m</t>
-  </si>
-  <si>
     <t>Km IMPORT</t>
   </si>
   <si>
-    <t>257 km</t>
+    <t>100</t>
   </si>
   <si>
     <t>REQUESTED HEIGHT OF THE TRUCK</t>
   </si>
   <si>
-    <t>2.61 m</t>
+    <t>adsa</t>
   </si>
   <si>
     <t>REQUESTED LENGTH OF THE TRUCK FIELD 1</t>
   </si>
   <si>
-    <t>11 m</t>
+    <t>asdasd</t>
   </si>
   <si>
     <t>REQUESTED LENGTH OF THE TRUCK FIELD 2</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -504,9 +498,9 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.15234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.515625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="40.02734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="8.55078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="7.1796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2" s="1" customFormat="true">
@@ -543,37 +537,37 @@
         <v>7</v>
       </c>
       <c r="F6" t="s" s="16">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="16">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="C7" t="s" s="16">
+      <c r="E7" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="E7" t="s" s="16">
+      <c r="F7" t="s" s="16">
         <v>11</v>
-      </c>
-      <c r="F7" t="s" s="16">
-        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="E8" t="s" s="16">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s" s="16">
         <v>13</v>
-      </c>
-      <c r="F8" t="s" s="16">
-        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="E9" t="s" s="16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s" s="16">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>